<commit_message>
changing jitter figure size
</commit_message>
<xml_diff>
--- a/FishLandings/household groups/statistics.xlsx
+++ b/FishLandings/household groups/statistics.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmmaStrand\MyProjects\Kenya_SamakiSalama\FishLandings\household groups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0B558A7-9AF6-408C-90E7-E01DE9F951EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B51207-FD09-4A4A-AE6E-1DB6919A0064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27615" yWindow="2790" windowWidth="21600" windowHeight="13170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29415" yWindow="3210" windowWidth="20730" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -89,7 +89,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -120,7 +120,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -133,6 +133,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -267,21 +273,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -299,6 +304,15 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -584,7 +598,7 @@
   <dimension ref="B3:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -595,293 +609,291 @@
     <col min="4" max="4" width="10.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="10" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G3" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>23597.200000000001</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>498.32799999999997</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="21">
         <v>2</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="21">
         <v>1297.0999999999999</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="21">
         <v>13.696</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="22" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="4"/>
-      <c r="C6" s="2" t="s">
+      <c r="B6" s="3"/>
+      <c r="C6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>229</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>10843.8</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="3"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="4"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="17" t="s">
+      <c r="B7" s="3"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="17" t="s">
+      <c r="E7" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="F7" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="17" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B8" s="4"/>
-      <c r="C8" s="2" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D8" s="4">
         <v>-2.4235549999999999</v>
       </c>
-      <c r="E8" s="5">
+      <c r="E8" s="4">
         <v>-5.3664601000000003</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>0.51934990000000003</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>0.12914929999999999</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B9" s="4"/>
-      <c r="C9" s="2" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="4">
         <v>2.9294389999999999</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="4">
         <v>-0.23874029999999999</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>6.0976172999999996</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>7.6556100000000002E-2</v>
       </c>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="7"/>
-      <c r="C10" s="8" t="s">
+      <c r="B10" s="6"/>
+      <c r="C10" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="19">
         <v>5.3529939999999998</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="19">
         <v>2.9357253000000001</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="19">
         <v>7.7702619999999998</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="20" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="15" t="s">
+      <c r="G12" s="14" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="12"/>
-      <c r="C13" s="2" t="s">
+      <c r="B13" s="11"/>
+      <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>1</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>23597.200000000001</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>498.32799999999997</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>2</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>1297.0999999999999</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>13.696</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B15" s="4"/>
-      <c r="C15" s="2" t="s">
+      <c r="B15" s="3"/>
+      <c r="C15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>229</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>10843.8</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="3"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="4"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="17" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="17" t="s">
+      <c r="E16" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="17" t="s">
+      <c r="F16" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="17" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B17" s="4"/>
-      <c r="C17" s="2" t="s">
+      <c r="B17" s="3"/>
+      <c r="C17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>-2.4235549999999999</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>-5.3664601000000003</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <v>0.51934990000000003</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <v>0.12914929999999999</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B18" s="4"/>
-      <c r="C18" s="2" t="s">
+      <c r="B18" s="3"/>
+      <c r="C18" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D18" s="4">
         <v>2.9294389999999999</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="4">
         <v>-0.23874029999999999</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="4">
         <v>6.0976172999999996</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="5">
         <v>7.6556100000000002E-2</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B19" s="7"/>
-      <c r="C19" s="8" t="s">
+      <c r="B19" s="6"/>
+      <c r="C19" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="8">
         <v>5.3529939999999998</v>
       </c>
-      <c r="E19" s="9">
+      <c r="E19" s="8">
         <v>2.9357253000000001</v>
       </c>
-      <c r="F19" s="9">
+      <c r="F19" s="8">
         <v>7.7702619999999998</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="9" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
distance from maturity plot and stats
</commit_message>
<xml_diff>
--- a/FishLandings/household groups/statistics.xlsx
+++ b/FishLandings/household groups/statistics.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EmmaStrand\MyProjects\Kenya_SamakiSalama\FishLandings\household groups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B51207-FD09-4A4A-AE6E-1DB6919A0064}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFCBA00B-F722-4A2A-8880-D40D1F1DBC8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29415" yWindow="3210" windowWidth="20730" windowHeight="12510" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="20">
   <si>
     <t>Effect</t>
   </si>
@@ -82,6 +82,9 @@
   </si>
   <si>
     <t>aov (length ~ group)</t>
+  </si>
+  <si>
+    <t>Distance from Lmat (cm)</t>
   </si>
 </sst>
 </file>
@@ -273,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -285,11 +288,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -313,6 +311,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -598,7 +602,7 @@
   <dimension ref="B3:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -609,32 +613,32 @@
     <col min="4" max="4" width="10.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.21875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" style="10" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="7" customWidth="1"/>
     <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -657,19 +661,19 @@
       <c r="B5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="21" t="s">
+      <c r="C5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="18">
         <v>2</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="18">
         <v>1297.0999999999999</v>
       </c>
-      <c r="F5" s="21">
+      <c r="F5" s="18">
         <v>13.696</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="19" t="s">
         <v>17</v>
       </c>
     </row>
@@ -688,17 +692,17 @@
     </row>
     <row r="7" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="3"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="16" t="s">
+      <c r="C7" s="12"/>
+      <c r="D7" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="14" t="s">
         <v>12</v>
       </c>
     </row>
@@ -740,44 +744,46 @@
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B10" s="6"/>
-      <c r="C10" s="18" t="s">
+      <c r="C10" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="16">
         <v>5.3529939999999998</v>
       </c>
-      <c r="E10" s="19">
+      <c r="E10" s="16">
         <v>2.9357253000000001</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="16">
         <v>7.7702619999999998</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="17" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F12" s="13" t="s">
+      <c r="F12" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B13" s="11"/>
+      <c r="B13" s="8" t="s">
+        <v>19</v>
+      </c>
       <c r="C13" s="1" t="s">
         <v>15</v>
       </c>
@@ -785,33 +791,33 @@
         <v>1</v>
       </c>
       <c r="E13" s="1">
-        <v>23597.200000000001</v>
+        <v>308.39999999999998</v>
       </c>
       <c r="F13" s="1">
-        <v>498.32799999999997</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>17</v>
+        <v>6.7995000000000001</v>
+      </c>
+      <c r="G13" s="5">
+        <v>9.7179999999999992E-3</v>
       </c>
     </row>
     <row r="14" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="18">
         <v>2</v>
       </c>
-      <c r="E14" s="1">
-        <v>1297.0999999999999</v>
-      </c>
-      <c r="F14" s="1">
-        <v>13.696</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>17</v>
+      <c r="E14" s="18">
+        <v>471.2</v>
+      </c>
+      <c r="F14" s="18">
+        <v>5.1947999999999999</v>
+      </c>
+      <c r="G14" s="21">
+        <v>6.2170000000000003E-3</v>
       </c>
     </row>
     <row r="15" spans="2:7" x14ac:dyDescent="0.3">
@@ -823,23 +829,23 @@
         <v>229</v>
       </c>
       <c r="E15" s="1">
-        <v>10843.8</v>
+        <v>10386.5</v>
       </c>
       <c r="G15" s="2"/>
     </row>
     <row r="16" spans="2:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="3"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="16" t="s">
+      <c r="C16" s="12"/>
+      <c r="D16" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="16" t="s">
+      <c r="E16" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="14" t="s">
         <v>12</v>
       </c>
     </row>
@@ -849,16 +855,16 @@
         <v>6</v>
       </c>
       <c r="D17" s="4">
-        <v>-2.4235549999999999</v>
+        <v>-2.50353</v>
       </c>
       <c r="E17" s="4">
-        <v>-5.3664601000000003</v>
+        <v>-5.3837223999999999</v>
       </c>
       <c r="F17" s="4">
-        <v>0.51934990000000003</v>
+        <v>0.37665149999999997</v>
       </c>
       <c r="G17" s="5">
-        <v>0.12914929999999999</v>
+        <v>0.1026784</v>
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.3">
@@ -867,34 +873,34 @@
         <v>7</v>
       </c>
       <c r="D18" s="4">
-        <v>2.9294389999999999</v>
+        <v>0.50990000000000002</v>
       </c>
       <c r="E18" s="4">
-        <v>-0.23874029999999999</v>
+        <v>-2.5907192000000001</v>
       </c>
       <c r="F18" s="4">
-        <v>6.0976172999999996</v>
+        <v>3.6106004</v>
       </c>
       <c r="G18" s="5">
-        <v>7.6556100000000002E-2</v>
+        <v>0.92041379999999995</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B19" s="6"/>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="D19" s="8">
-        <v>5.3529939999999998</v>
-      </c>
-      <c r="E19" s="8">
-        <v>2.9357253000000001</v>
-      </c>
-      <c r="F19" s="8">
-        <v>7.7702619999999998</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>17</v>
+      <c r="D19" s="16">
+        <v>3.0134759999999998</v>
+      </c>
+      <c r="E19" s="16">
+        <v>0.64772359999999995</v>
+      </c>
+      <c r="F19" s="16">
+        <v>5.3792285</v>
+      </c>
+      <c r="G19" s="20">
+        <v>8.2707000000000006E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>